<commit_message>
explored different number of topics for LDA, ran BERTopic
</commit_message>
<xml_diff>
--- a/topics_per_model.xlsx
+++ b/topics_per_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimsagha/Documents/Projects/NLP_Topic_Extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755467F7-ECD3-8647-8ED0-9F731A812EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAC44B5-64B1-9745-8E9E-0D33598DF88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{79F22EE7-A633-B441-A412-EC3E637107D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>NER</t>
   </si>
@@ -45,21 +45,9 @@
     <t>BERTopic</t>
   </si>
   <si>
-    <t>Trump, Clinton, Obama, president, Russia</t>
-  </si>
-  <si>
-    <t>Trump, Clinton, Campaign, state</t>
-  </si>
-  <si>
     <t>Trump, police, clinton, president</t>
   </si>
   <si>
-    <t>Trump, breitbart, clinton, gun, company, woman</t>
-  </si>
-  <si>
-    <t>Trump, Clinton, president, campaign, republican</t>
-  </si>
-  <si>
     <t>LDA (10 topics)</t>
   </si>
   <si>
@@ -97,14 +85,40 @@
   </si>
   <si>
     <t>last year surpassed queen victoria, london — queen elizabeth ii, first time since 1988, christmas day church service</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>Trump, Clinton</t>
+  </si>
+  <si>
+    <t>Trump, police</t>
+  </si>
+  <si>
+    <t>Trump, police, Clinton</t>
+  </si>
+  <si>
+    <t>Trump, Clinton, president</t>
+  </si>
+  <si>
+    <t>geopolitics (and outliers)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -128,12 +142,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,114 +508,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F3C714-34CB-544D-A17A-82746F624A05}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="110.33203125" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>